<commit_message>
Ajusta configs do Kafka
</commit_message>
<xml_diff>
--- a/Conteúdos/Mapeamento dos Tópicos.xlsx
+++ b/Conteúdos/Mapeamento dos Tópicos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Área de Trabalho\Projetos\Curso Saga Outbox\Curso Outbox Saga Orquestrado\Conteúdos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1940E1F2-00FF-4F03-95CE-0C84F9B3E1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EDD745-85B2-419F-B6F8-5B5DEA536D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9615" yWindow="2295" windowWidth="17250" windowHeight="8865" xr2:uid="{BF5BEBC6-FA3F-460D-8800-6EAA4BFD5AB2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BF5BEBC6-FA3F-460D-8800-6EAA4BFD5AB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -587,21 +587,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738384B0-AF7B-464E-A311-A3F99F9EF50B}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -611,17 +613,17 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -631,17 +633,17 @@
       <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -651,17 +653,17 @@
       <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>28</v>
       </c>
@@ -671,17 +673,17 @@
       <c r="C4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="G4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>28</v>
       </c>
@@ -691,17 +693,17 @@
       <c r="C5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="G5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>28</v>
       </c>
@@ -711,17 +713,17 @@
       <c r="C6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>32</v>
       </c>
@@ -731,17 +733,17 @@
       <c r="C7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>32</v>
       </c>
@@ -751,17 +753,17 @@
       <c r="C8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="F8" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>32</v>
       </c>
@@ -771,17 +773,17 @@
       <c r="C9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="F9" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="G9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
@@ -791,17 +793,17 @@
       <c r="C10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="F10" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="G10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>33</v>
       </c>
@@ -811,17 +813,17 @@
       <c r="C11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="F11" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="G11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>33</v>
       </c>
@@ -831,57 +833,57 @@
       <c r="C12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="F12" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F13" s="8" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="F13" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="G13" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F15" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F16" s="10" t="s">
-        <v>20</v>
-      </c>
       <c r="G16" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="11" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>